<commit_message>
Organize project: Consolidate application code and client documentation
</commit_message>
<xml_diff>
--- a/backend/exports/competitors_export.xlsx
+++ b/backend/exports/competitors_export.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF97"/>
+  <dimension ref="A1:AF98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -661,7 +661,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -973,7 +973,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F7" s="2" t="n"/>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F10" s="2" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F11" s="2" t="n"/>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F12" s="2" t="n"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F15" s="2" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F16" s="2" t="n"/>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F17" s="2" t="n"/>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F18" s="2" t="n"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F19" s="2" t="n"/>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F21" s="2" t="n"/>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F22" s="2" t="n"/>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F23" s="2" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F24" s="2" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F26" s="2" t="n"/>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F27" s="2" t="n"/>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F28" s="2" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F29" s="2" t="n"/>
@@ -5029,7 +5029,7 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F30" s="2" t="n"/>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F31" s="2" t="n"/>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F33" s="2" t="n"/>
@@ -5653,7 +5653,7 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F34" s="2" t="n"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F35" s="2" t="n"/>
@@ -5965,7 +5965,7 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F36" s="2" t="n"/>
@@ -6121,7 +6121,7 @@
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F37" s="2" t="n"/>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F38" s="2" t="n"/>
@@ -6433,7 +6433,7 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F39" s="2" t="n"/>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F40" s="2" t="n"/>
@@ -6745,7 +6745,7 @@
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F41" s="2" t="n"/>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F42" s="2" t="n"/>
@@ -7057,7 +7057,7 @@
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F43" s="2" t="n"/>
@@ -7213,7 +7213,7 @@
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F44" s="2" t="n"/>
@@ -7369,7 +7369,7 @@
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F45" s="2" t="n"/>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F46" s="2" t="n"/>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F48" s="2" t="n"/>
@@ -7993,7 +7993,7 @@
       </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
@@ -8149,7 +8149,7 @@
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F50" s="2" t="n"/>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F51" s="2" t="n"/>
@@ -8461,7 +8461,7 @@
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F52" s="2" t="n"/>
@@ -8617,7 +8617,7 @@
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F53" s="2" t="n"/>
@@ -8773,7 +8773,7 @@
       </c>
       <c r="E54" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F54" s="2" t="n"/>
@@ -8929,7 +8929,7 @@
       </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F55" s="2" t="n"/>
@@ -9085,7 +9085,7 @@
       </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F56" s="2" t="n"/>
@@ -9241,7 +9241,7 @@
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F57" s="2" t="n"/>
@@ -9397,7 +9397,7 @@
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F58" s="2" t="n"/>
@@ -9553,7 +9553,7 @@
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F59" s="2" t="n"/>
@@ -9709,7 +9709,7 @@
       </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F60" s="2" t="n"/>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F61" s="2" t="n"/>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F62" s="2" t="n"/>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F63" s="2" t="n"/>
@@ -10333,7 +10333,7 @@
       </c>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F64" s="2" t="n"/>
@@ -10489,7 +10489,7 @@
       </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F65" s="2" t="n"/>
@@ -10645,7 +10645,7 @@
       </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F66" s="2" t="n"/>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="E68" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F68" s="2" t="n"/>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F69" s="2" t="n"/>
@@ -11269,7 +11269,7 @@
       </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F70" s="2" t="n"/>
@@ -11425,7 +11425,7 @@
       </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F71" s="2" t="n"/>
@@ -11581,7 +11581,7 @@
       </c>
       <c r="E72" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F72" s="2" t="n"/>
@@ -11737,7 +11737,7 @@
       </c>
       <c r="E73" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F73" s="2" t="n"/>
@@ -11893,7 +11893,7 @@
       </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F74" s="2" t="n"/>
@@ -12049,7 +12049,7 @@
       </c>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F75" s="2" t="n"/>
@@ -12205,7 +12205,7 @@
       </c>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F76" s="2" t="n"/>
@@ -12361,7 +12361,7 @@
       </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F77" s="2" t="n"/>
@@ -12517,7 +12517,7 @@
       </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F78" s="2" t="n"/>
@@ -12829,7 +12829,7 @@
       </c>
       <c r="E80" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F80" s="2" t="n"/>
@@ -12985,7 +12985,7 @@
       </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F81" s="2" t="n"/>
@@ -13141,7 +13141,7 @@
       </c>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F82" s="2" t="n"/>
@@ -13297,7 +13297,7 @@
       </c>
       <c r="E83" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F83" s="2" t="n"/>
@@ -13609,7 +13609,7 @@
       </c>
       <c r="E85" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F85" s="2" t="n"/>
@@ -13765,7 +13765,7 @@
       </c>
       <c r="E86" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F86" s="2" t="n"/>
@@ -13921,7 +13921,7 @@
       </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F87" s="2" t="n"/>
@@ -13975,7 +13975,7 @@
       </c>
       <c r="E88" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F88" s="2" t="inlineStr">
@@ -14011,15 +14011,35 @@
       <c r="AF88" s="2" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n"/>
-      <c r="B89" s="2" t="n"/>
-      <c r="C89" s="2" t="n"/>
-      <c r="D89" s="2" t="n"/>
-      <c r="E89" s="2" t="n"/>
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t>Phreesia Audit</t>
+        </is>
+      </c>
+      <c r="B89" s="2" t="inlineStr">
+        <is>
+          <t>https://phreesia.com</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
       <c r="F89" s="2" t="n"/>
       <c r="G89" s="2" t="n"/>
-      <c r="H89" s="2" t="n"/>
-      <c r="I89" s="2" t="n"/>
+      <c r="H89" s="2" t="inlineStr"/>
+      <c r="I89" s="2" t="inlineStr"/>
       <c r="J89" s="2" t="n"/>
       <c r="K89" s="2" t="n"/>
       <c r="L89" s="2" t="n"/>
@@ -14316,6 +14336,40 @@
       <c r="AE97" s="2" t="n"/>
       <c r="AF97" s="2" t="n"/>
     </row>
+    <row r="98">
+      <c r="A98" s="2" t="n"/>
+      <c r="B98" s="2" t="n"/>
+      <c r="C98" s="2" t="n"/>
+      <c r="D98" s="2" t="n"/>
+      <c r="E98" s="2" t="n"/>
+      <c r="F98" s="2" t="n"/>
+      <c r="G98" s="2" t="n"/>
+      <c r="H98" s="2" t="n"/>
+      <c r="I98" s="2" t="n"/>
+      <c r="J98" s="2" t="n"/>
+      <c r="K98" s="2" t="n"/>
+      <c r="L98" s="2" t="n"/>
+      <c r="M98" s="2" t="n"/>
+      <c r="N98" s="2" t="n"/>
+      <c r="O98" s="2" t="n"/>
+      <c r="P98" s="2" t="n"/>
+      <c r="Q98" s="2" t="n"/>
+      <c r="R98" s="2" t="n"/>
+      <c r="S98" s="2" t="n"/>
+      <c r="T98" s="2" t="n"/>
+      <c r="U98" s="2" t="n"/>
+      <c r="V98" s="2" t="n"/>
+      <c r="W98" s="2" t="n"/>
+      <c r="X98" s="2" t="n"/>
+      <c r="Y98" s="2" t="n"/>
+      <c r="Z98" s="2" t="n"/>
+      <c r="AA98" s="2" t="n"/>
+      <c r="AB98" s="2" t="n"/>
+      <c r="AC98" s="2" t="n"/>
+      <c r="AD98" s="2" t="n"/>
+      <c r="AE98" s="2" t="n"/>
+      <c r="AF98" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bugs: Add favicon, fix analytics charts script, update build scripts
</commit_message>
<xml_diff>
--- a/backend/exports/competitors_export.xlsx
+++ b/backend/exports/competitors_export.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF98"/>
+  <dimension ref="A1:AF99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14065,15 +14065,35 @@
       <c r="AF89" s="2" t="n"/>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n"/>
-      <c r="B90" s="2" t="n"/>
-      <c r="C90" s="2" t="n"/>
-      <c r="D90" s="2" t="n"/>
-      <c r="E90" s="2" t="n"/>
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>Test Corp</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
       <c r="F90" s="2" t="n"/>
       <c r="G90" s="2" t="n"/>
-      <c r="H90" s="2" t="n"/>
-      <c r="I90" s="2" t="n"/>
+      <c r="H90" s="2" t="inlineStr"/>
+      <c r="I90" s="2" t="inlineStr"/>
       <c r="J90" s="2" t="n"/>
       <c r="K90" s="2" t="n"/>
       <c r="L90" s="2" t="n"/>
@@ -14370,6 +14390,40 @@
       <c r="AE98" s="2" t="n"/>
       <c r="AF98" s="2" t="n"/>
     </row>
+    <row r="99">
+      <c r="A99" s="2" t="n"/>
+      <c r="B99" s="2" t="n"/>
+      <c r="C99" s="2" t="n"/>
+      <c r="D99" s="2" t="n"/>
+      <c r="E99" s="2" t="n"/>
+      <c r="F99" s="2" t="n"/>
+      <c r="G99" s="2" t="n"/>
+      <c r="H99" s="2" t="n"/>
+      <c r="I99" s="2" t="n"/>
+      <c r="J99" s="2" t="n"/>
+      <c r="K99" s="2" t="n"/>
+      <c r="L99" s="2" t="n"/>
+      <c r="M99" s="2" t="n"/>
+      <c r="N99" s="2" t="n"/>
+      <c r="O99" s="2" t="n"/>
+      <c r="P99" s="2" t="n"/>
+      <c r="Q99" s="2" t="n"/>
+      <c r="R99" s="2" t="n"/>
+      <c r="S99" s="2" t="n"/>
+      <c r="T99" s="2" t="n"/>
+      <c r="U99" s="2" t="n"/>
+      <c r="V99" s="2" t="n"/>
+      <c r="W99" s="2" t="n"/>
+      <c r="X99" s="2" t="n"/>
+      <c r="Y99" s="2" t="n"/>
+      <c r="Z99" s="2" t="n"/>
+      <c r="AA99" s="2" t="n"/>
+      <c r="AB99" s="2" t="n"/>
+      <c r="AC99" s="2" t="n"/>
+      <c r="AD99" s="2" t="n"/>
+      <c r="AE99" s="2" t="n"/>
+      <c r="AF99" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UI Finalization: Competitor Card Layout, Modal Fixes, News Feed Repair
</commit_message>
<xml_diff>
--- a/backend/exports/competitors_export.xlsx
+++ b/backend/exports/competitors_export.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF99"/>
+  <dimension ref="A1:AF100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13941,7 +13941,11 @@
       <c r="T87" s="2" t="n"/>
       <c r="U87" s="2" t="n"/>
       <c r="V87" s="2" t="n"/>
-      <c r="W87" s="2" t="n"/>
+      <c r="W87" s="2" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
       <c r="X87" s="2" t="n"/>
       <c r="Y87" s="2" t="n"/>
       <c r="Z87" s="2" t="n"/>
@@ -13999,7 +14003,11 @@
       <c r="T88" s="2" t="n"/>
       <c r="U88" s="2" t="n"/>
       <c r="V88" s="2" t="n"/>
-      <c r="W88" s="2" t="n"/>
+      <c r="W88" s="2" t="inlineStr">
+        <is>
+          <t>18%</t>
+        </is>
+      </c>
       <c r="X88" s="2" t="n"/>
       <c r="Y88" s="2" t="n"/>
       <c r="Z88" s="2" t="n"/>
@@ -14053,7 +14061,11 @@
       <c r="T89" s="2" t="n"/>
       <c r="U89" s="2" t="n"/>
       <c r="V89" s="2" t="n"/>
-      <c r="W89" s="2" t="n"/>
+      <c r="W89" s="2" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
       <c r="X89" s="2" t="n"/>
       <c r="Y89" s="2" t="n"/>
       <c r="Z89" s="2" t="n"/>
@@ -14107,7 +14119,11 @@
       <c r="T90" s="2" t="n"/>
       <c r="U90" s="2" t="n"/>
       <c r="V90" s="2" t="n"/>
-      <c r="W90" s="2" t="n"/>
+      <c r="W90" s="2" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
       <c r="X90" s="2" t="n"/>
       <c r="Y90" s="2" t="n"/>
       <c r="Z90" s="2" t="n"/>
@@ -14119,15 +14135,35 @@
       <c r="AF90" s="2" t="n"/>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n"/>
-      <c r="B91" s="2" t="n"/>
-      <c r="C91" s="2" t="n"/>
-      <c r="D91" s="2" t="n"/>
-      <c r="E91" s="2" t="n"/>
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
       <c r="F91" s="2" t="n"/>
       <c r="G91" s="2" t="n"/>
-      <c r="H91" s="2" t="n"/>
-      <c r="I91" s="2" t="n"/>
+      <c r="H91" s="2" t="inlineStr"/>
+      <c r="I91" s="2" t="inlineStr"/>
       <c r="J91" s="2" t="n"/>
       <c r="K91" s="2" t="n"/>
       <c r="L91" s="2" t="n"/>
@@ -14141,7 +14177,11 @@
       <c r="T91" s="2" t="n"/>
       <c r="U91" s="2" t="n"/>
       <c r="V91" s="2" t="n"/>
-      <c r="W91" s="2" t="n"/>
+      <c r="W91" s="2" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="X91" s="2" t="n"/>
       <c r="Y91" s="2" t="n"/>
       <c r="Z91" s="2" t="n"/>
@@ -14424,6 +14464,40 @@
       <c r="AE99" s="2" t="n"/>
       <c r="AF99" s="2" t="n"/>
     </row>
+    <row r="100">
+      <c r="A100" s="2" t="n"/>
+      <c r="B100" s="2" t="n"/>
+      <c r="C100" s="2" t="n"/>
+      <c r="D100" s="2" t="n"/>
+      <c r="E100" s="2" t="n"/>
+      <c r="F100" s="2" t="n"/>
+      <c r="G100" s="2" t="n"/>
+      <c r="H100" s="2" t="n"/>
+      <c r="I100" s="2" t="n"/>
+      <c r="J100" s="2" t="n"/>
+      <c r="K100" s="2" t="n"/>
+      <c r="L100" s="2" t="n"/>
+      <c r="M100" s="2" t="n"/>
+      <c r="N100" s="2" t="n"/>
+      <c r="O100" s="2" t="n"/>
+      <c r="P100" s="2" t="n"/>
+      <c r="Q100" s="2" t="n"/>
+      <c r="R100" s="2" t="n"/>
+      <c r="S100" s="2" t="n"/>
+      <c r="T100" s="2" t="n"/>
+      <c r="U100" s="2" t="n"/>
+      <c r="V100" s="2" t="n"/>
+      <c r="W100" s="2" t="n"/>
+      <c r="X100" s="2" t="n"/>
+      <c r="Y100" s="2" t="n"/>
+      <c r="Z100" s="2" t="n"/>
+      <c r="AA100" s="2" t="n"/>
+      <c r="AB100" s="2" t="n"/>
+      <c r="AC100" s="2" t="n"/>
+      <c r="AD100" s="2" t="n"/>
+      <c r="AE100" s="2" t="n"/>
+      <c r="AF100" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>